<commit_message>
Updated pinout on TEENSY IO MAP
</commit_message>
<xml_diff>
--- a/Teensy IO Map.xlsx
+++ b/Teensy IO Map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npb21\Desktop\School\FSAE Electric\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dcecee288486a0d5/Documents/Arduino/BEV_2021_Teensy_Firmware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E14BF5-301B-46B7-94DD-3D721CD815A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{CAC71B1E-86C1-4C54-AEDC-DA1FE7FE0A7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{099FCFAC-71AB-43FC-91A7-303E9D374233}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3015" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="119">
   <si>
     <t>GND</t>
   </si>
@@ -336,9 +336,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>0-5 SPARE</t>
-  </si>
-  <si>
     <t>add Can tx/rx</t>
   </si>
   <si>
@@ -373,6 +370,27 @@
   </si>
   <si>
     <t>reset</t>
+  </si>
+  <si>
+    <t>spare in</t>
+  </si>
+  <si>
+    <t>spare out</t>
+  </si>
+  <si>
+    <t>pwm/digital</t>
+  </si>
+  <si>
+    <t>CAN TRX</t>
+  </si>
+  <si>
+    <t>I2C TRX</t>
+  </si>
+  <si>
+    <t>analog</t>
+  </si>
+  <si>
+    <t>pwm</t>
   </si>
 </sst>
 </file>
@@ -587,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -610,21 +628,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -644,6 +647,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -929,60 +954,61 @@
   <dimension ref="A2:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="1" max="1" width="10.20703125" customWidth="1"/>
     <col min="21" max="21" width="32.3671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="11" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="13" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
       <c r="U2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="7" t="s">
@@ -997,7 +1023,7 @@
       <c r="J4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="8"/>
+      <c r="K4" s="15"/>
       <c r="L4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1032,7 +1058,7 @@
       <c r="J5" s="4">
         <v>0</v>
       </c>
-      <c r="K5" s="9"/>
+      <c r="K5" s="16"/>
       <c r="L5" s="5" t="s">
         <v>0</v>
       </c>
@@ -1065,7 +1091,7 @@
       <c r="J6" s="4">
         <v>1</v>
       </c>
-      <c r="K6" s="9"/>
+      <c r="K6" s="16"/>
       <c r="L6" s="5" t="s">
         <v>1</v>
       </c>
@@ -1102,7 +1128,7 @@
       <c r="J7" s="4">
         <v>2</v>
       </c>
-      <c r="K7" s="9"/>
+      <c r="K7" s="16"/>
       <c r="L7" s="5">
         <v>23</v>
       </c>
@@ -1119,14 +1145,20 @@
         <v>3</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
+      <c r="T7" s="21" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
       <c r="C8" s="7" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -1141,7 +1173,7 @@
       <c r="J8" s="4">
         <v>3</v>
       </c>
-      <c r="K8" s="9"/>
+      <c r="K8" s="16"/>
       <c r="L8" s="5">
         <v>22</v>
       </c>
@@ -1156,14 +1188,18 @@
         <v>3</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
+      <c r="T8" s="21"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
       <c r="C9" s="7" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -1178,7 +1214,7 @@
       <c r="J9" s="4">
         <v>4</v>
       </c>
-      <c r="K9" s="9"/>
+      <c r="K9" s="16"/>
       <c r="L9" s="5">
         <v>21</v>
       </c>
@@ -1193,14 +1229,20 @@
       </c>
       <c r="P9" s="3"/>
       <c r="Q9" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
+      <c r="T9" s="22" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>114</v>
+      </c>
       <c r="C10" s="7" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -1215,7 +1257,7 @@
       <c r="J10" s="4">
         <v>5</v>
       </c>
-      <c r="K10" s="9"/>
+      <c r="K10" s="16"/>
       <c r="L10" s="5">
         <v>20</v>
       </c>
@@ -1230,14 +1272,20 @@
       </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
+      <c r="T10" s="6" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
       <c r="C11" s="7" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1252,7 +1300,7 @@
       <c r="J11" s="4">
         <v>6</v>
       </c>
-      <c r="K11" s="9"/>
+      <c r="K11" s="16"/>
       <c r="L11" s="5">
         <v>19</v>
       </c>
@@ -1266,18 +1314,24 @@
       <c r="P11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q11" s="14" t="s">
+      <c r="Q11" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="R11" s="15"/>
-      <c r="S11" s="16"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="21" t="s">
+        <v>116</v>
+      </c>
       <c r="U11" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>114</v>
+      </c>
       <c r="C12" s="7" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1294,7 +1348,7 @@
       <c r="J12" s="4">
         <v>7</v>
       </c>
-      <c r="K12" s="9"/>
+      <c r="K12" s="16"/>
       <c r="L12" s="5">
         <v>18</v>
       </c>
@@ -1308,13 +1362,17 @@
       <c r="P12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="19"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="21"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>114</v>
+      </c>
       <c r="C13" s="7" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1331,7 +1389,7 @@
       <c r="J13" s="4">
         <v>8</v>
       </c>
-      <c r="K13" s="9"/>
+      <c r="K13" s="16"/>
       <c r="L13" s="5">
         <v>17</v>
       </c>
@@ -1346,14 +1404,23 @@
       </c>
       <c r="P13" s="3"/>
       <c r="Q13" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
+      <c r="T13" s="22" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="C14" s="7" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1368,7 +1435,7 @@
       <c r="J14" s="4">
         <v>9</v>
       </c>
-      <c r="K14" s="9"/>
+      <c r="K14" s="16"/>
       <c r="L14" s="5">
         <v>16</v>
       </c>
@@ -1383,14 +1450,24 @@
       </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
+      <c r="T14" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="U14" s="20"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="C15" s="7" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1407,7 +1484,7 @@
       <c r="J15" s="4">
         <v>10</v>
       </c>
-      <c r="K15" s="9"/>
+      <c r="K15" s="16"/>
       <c r="L15" s="5">
         <v>15</v>
       </c>
@@ -1423,21 +1500,20 @@
       <c r="P15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q15" s="7" t="s">
-        <v>85</v>
-      </c>
+      <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
-      <c r="T15" s="6" t="s">
+      <c r="U15" s="20"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="U15" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="C16" s="7" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -1454,7 +1530,7 @@
       <c r="J16" s="4">
         <v>11</v>
       </c>
-      <c r="K16" s="9"/>
+      <c r="K16" s="16"/>
       <c r="L16" s="5">
         <v>14</v>
       </c>
@@ -1471,20 +1547,24 @@
         <v>3</v>
       </c>
       <c r="Q16" s="7" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="R16" s="7"/>
       <c r="S16" s="7"/>
-      <c r="T16" s="6" t="s">
+      <c r="T16" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="U16" s="20"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="U16" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" s="7" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1501,7 +1581,7 @@
       <c r="J17" s="4">
         <v>12</v>
       </c>
-      <c r="K17" s="9"/>
+      <c r="K17" s="16"/>
       <c r="L17" s="5">
         <v>13</v>
       </c>
@@ -1515,17 +1595,10 @@
       <c r="P17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q17" s="7" t="s">
-        <v>87</v>
-      </c>
+      <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
       <c r="S17" s="7"/>
-      <c r="T17" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="U17" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="U17" s="20"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" s="7"/>
@@ -1538,7 +1611,7 @@
       <c r="J18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K18" s="9"/>
+      <c r="K18" s="16"/>
       <c r="L18" s="5" t="s">
         <v>0</v>
       </c>
@@ -1549,8 +1622,7 @@
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
       <c r="S18" s="7"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="6"/>
+      <c r="U18" s="20"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
@@ -1579,7 +1651,7 @@
       <c r="J19" s="4">
         <v>24</v>
       </c>
-      <c r="K19" s="9"/>
+      <c r="K19" s="16"/>
       <c r="L19" s="5">
         <v>41</v>
       </c>
@@ -1590,16 +1662,14 @@
       <c r="O19" s="2"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="7" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="R19" s="7"/>
       <c r="S19" s="7"/>
-      <c r="T19" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="U19" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="T19" t="s">
+        <v>117</v>
+      </c>
+      <c r="U19" s="20"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
@@ -1628,7 +1698,7 @@
       <c r="J20" s="4">
         <v>25</v>
       </c>
-      <c r="K20" s="9"/>
+      <c r="K20" s="16"/>
       <c r="L20" s="5">
         <v>40</v>
       </c>
@@ -1638,9 +1708,15 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="3"/>
-      <c r="Q20" s="7"/>
+      <c r="Q20" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="R20" s="7"/>
       <c r="S20" s="7"/>
+      <c r="T20" t="s">
+        <v>117</v>
+      </c>
+      <c r="U20" s="20"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
@@ -1665,7 +1741,7 @@
       <c r="J21" s="4">
         <v>26</v>
       </c>
-      <c r="K21" s="9"/>
+      <c r="K21" s="16"/>
       <c r="L21" s="5">
         <v>39</v>
       </c>
@@ -1679,9 +1755,14 @@
         <v>11</v>
       </c>
       <c r="P21" s="3"/>
-      <c r="Q21" s="7"/>
+      <c r="Q21" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="R21" s="7"/>
       <c r="S21" s="7"/>
+      <c r="T21" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="C22" s="7"/>
@@ -1698,7 +1779,7 @@
       <c r="J22" s="4">
         <v>27</v>
       </c>
-      <c r="K22" s="9"/>
+      <c r="K22" s="16"/>
       <c r="L22" s="5">
         <v>38</v>
       </c>
@@ -1712,9 +1793,14 @@
         <v>12</v>
       </c>
       <c r="P22" s="3"/>
-      <c r="Q22" s="7"/>
+      <c r="Q22" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="R22" s="7"/>
       <c r="S22" s="7"/>
+      <c r="T22" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="C23" s="7"/>
@@ -1731,7 +1817,7 @@
       <c r="J23" s="4">
         <v>28</v>
       </c>
-      <c r="K23" s="9"/>
+      <c r="K23" s="16"/>
       <c r="L23" s="5">
         <v>37</v>
       </c>
@@ -1749,7 +1835,7 @@
       <c r="R23" s="7"/>
       <c r="S23" s="7"/>
       <c r="T23" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="U23" s="6" t="s">
         <v>99</v>
@@ -1770,7 +1856,7 @@
       <c r="J24" s="4">
         <v>29</v>
       </c>
-      <c r="K24" s="9"/>
+      <c r="K24" s="16"/>
       <c r="L24" s="5">
         <v>36</v>
       </c>
@@ -1783,7 +1869,7 @@
         <v>3</v>
       </c>
       <c r="Q24" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R24" s="7"/>
       <c r="S24" s="7"/>
@@ -1807,7 +1893,7 @@
       <c r="J25" s="4">
         <v>30</v>
       </c>
-      <c r="K25" s="9"/>
+      <c r="K25" s="16"/>
       <c r="L25" s="5">
         <v>35</v>
       </c>
@@ -1834,7 +1920,7 @@
       <c r="J26" s="4">
         <v>31</v>
       </c>
-      <c r="K26" s="9"/>
+      <c r="K26" s="16"/>
       <c r="L26" s="5">
         <v>34</v>
       </c>
@@ -1861,7 +1947,7 @@
       <c r="J27" s="4">
         <v>32</v>
       </c>
-      <c r="K27" s="10"/>
+      <c r="K27" s="17"/>
       <c r="L27" s="5">
         <v>33</v>
       </c>
@@ -1879,31 +1965,68 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="U28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="U29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="U30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="U31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="U32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="51">
+  <mergeCells count="53">
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F2:P3"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="K4:K27"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
     <mergeCell ref="Q27:S27"/>
     <mergeCell ref="Q2:S3"/>
     <mergeCell ref="C2:E3"/>
@@ -1914,47 +2037,12 @@
     <mergeCell ref="Q24:S24"/>
     <mergeCell ref="Q25:S25"/>
     <mergeCell ref="Q26:S26"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="Q14:S14"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C15:E15"/>
-    <mergeCell ref="K4:K27"/>
-    <mergeCell ref="F2:P3"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C27:E27"/>
     <mergeCell ref="C16:E16"/>
+    <mergeCell ref="Q18:S18"/>
     <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="Q20:S20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the teensy map to reflect the meeting from 2/5/21
</commit_message>
<xml_diff>
--- a/Teensy IO Map.xlsx
+++ b/Teensy IO Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dcecee288486a0d5/Documents/Arduino/BEV_2021_Teensy_Firmware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{CAC71B1E-86C1-4C54-AEDC-DA1FE7FE0A7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{099FCFAC-71AB-43FC-91A7-303E9D374233}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{CAC71B1E-86C1-4C54-AEDC-DA1FE7FE0A7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A7C5CCF0-D951-41F3-A134-FE8941946192}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="3015" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="124">
   <si>
     <t>GND</t>
   </si>
@@ -391,6 +391,21 @@
   </si>
   <si>
     <t>pwm</t>
+  </si>
+  <si>
+    <t>current in</t>
+  </si>
+  <si>
+    <t>0-5</t>
+  </si>
+  <si>
+    <t>current out</t>
+  </si>
+  <si>
+    <t>wheel move out</t>
+  </si>
+  <si>
+    <t>12v</t>
   </si>
 </sst>
 </file>
@@ -625,7 +640,29 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -647,28 +684,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -954,7 +969,7 @@
   <dimension ref="A2:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+      <selection activeCell="U13" sqref="U13:U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -964,58 +979,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="18" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="8" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
       <c r="U2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1023,7 +1038,7 @@
       <c r="J4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="15"/>
+      <c r="K4" s="13"/>
       <c r="L4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1033,16 +1048,16 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="3"/>
-      <c r="Q4" s="7" t="s">
+      <c r="Q4" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1058,7 +1073,7 @@
       <c r="J5" s="4">
         <v>0</v>
       </c>
-      <c r="K5" s="16"/>
+      <c r="K5" s="14"/>
       <c r="L5" s="5" t="s">
         <v>0</v>
       </c>
@@ -1066,16 +1081,16 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="3"/>
-      <c r="Q5" s="7" t="s">
+      <c r="Q5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1091,7 +1106,7 @@
       <c r="J6" s="4">
         <v>1</v>
       </c>
-      <c r="K6" s="16"/>
+      <c r="K6" s="14"/>
       <c r="L6" s="5" t="s">
         <v>1</v>
       </c>
@@ -1101,9 +1116,9 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="3"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
@@ -1112,11 +1127,11 @@
       <c r="B7" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1128,7 +1143,7 @@
       <c r="J7" s="4">
         <v>2</v>
       </c>
-      <c r="K7" s="16"/>
+      <c r="K7" s="14"/>
       <c r="L7" s="5">
         <v>23</v>
       </c>
@@ -1144,24 +1159,27 @@
       <c r="P7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q7" s="7" t="s">
+      <c r="Q7" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="21" t="s">
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="10" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1173,7 +1191,7 @@
       <c r="J8" s="4">
         <v>3</v>
       </c>
-      <c r="K8" s="16"/>
+      <c r="K8" s="14"/>
       <c r="L8" s="5">
         <v>22</v>
       </c>
@@ -1187,22 +1205,25 @@
       <c r="P8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q8" s="7" t="s">
+      <c r="Q8" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="21"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="10"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+        <v>94</v>
+      </c>
+      <c r="B9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1214,7 +1235,7 @@
       <c r="J9" s="4">
         <v>4</v>
       </c>
-      <c r="K9" s="16"/>
+      <c r="K9" s="14"/>
       <c r="L9" s="5">
         <v>21</v>
       </c>
@@ -1228,24 +1249,27 @@
         <v>69</v>
       </c>
       <c r="P9" s="3"/>
-      <c r="Q9" s="7" t="s">
+      <c r="Q9" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="22" t="s">
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="8" t="s">
         <v>117</v>
+      </c>
+      <c r="U9" s="8" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>114</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1257,7 +1281,7 @@
       <c r="J10" s="4">
         <v>5</v>
       </c>
-      <c r="K10" s="16"/>
+      <c r="K10" s="14"/>
       <c r="L10" s="5">
         <v>20</v>
       </c>
@@ -1271,24 +1295,27 @@
         <v>70</v>
       </c>
       <c r="P10" s="3"/>
-      <c r="Q10" s="7" t="s">
+      <c r="Q10" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
       <c r="T10" s="6" t="s">
         <v>117</v>
+      </c>
+      <c r="U10" s="8" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>114</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="1" t="s">
         <v>3</v>
       </c>
@@ -1300,7 +1327,7 @@
       <c r="J11" s="4">
         <v>6</v>
       </c>
-      <c r="K11" s="16"/>
+      <c r="K11" s="14"/>
       <c r="L11" s="5">
         <v>19</v>
       </c>
@@ -1314,12 +1341,12 @@
       <c r="P11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q11" s="9" t="s">
+      <c r="Q11" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="R11" s="10"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="21" t="s">
+      <c r="R11" s="18"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="10" t="s">
         <v>116</v>
       </c>
       <c r="U11" t="s">
@@ -1330,11 +1357,11 @@
       <c r="A12" t="s">
         <v>114</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1348,7 +1375,7 @@
       <c r="J12" s="4">
         <v>7</v>
       </c>
-      <c r="K12" s="16"/>
+      <c r="K12" s="14"/>
       <c r="L12" s="5">
         <v>18</v>
       </c>
@@ -1362,20 +1389,20 @@
       <c r="P12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="21"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="10"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="1" t="s">
         <v>3</v>
       </c>
@@ -1389,7 +1416,7 @@
       <c r="J13" s="4">
         <v>8</v>
       </c>
-      <c r="K13" s="16"/>
+      <c r="K13" s="14"/>
       <c r="L13" s="5">
         <v>17</v>
       </c>
@@ -1403,13 +1430,16 @@
         <v>73</v>
       </c>
       <c r="P13" s="3"/>
-      <c r="Q13" s="7" t="s">
+      <c r="Q13" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="22" t="s">
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="8" t="s">
         <v>117</v>
+      </c>
+      <c r="U13" s="8" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -1419,11 +1449,11 @@
       <c r="B14" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1435,7 +1465,7 @@
       <c r="J14" s="4">
         <v>9</v>
       </c>
-      <c r="K14" s="16"/>
+      <c r="K14" s="14"/>
       <c r="L14" s="5">
         <v>16</v>
       </c>
@@ -1449,15 +1479,17 @@
         <v>74</v>
       </c>
       <c r="P14" s="3"/>
-      <c r="Q14" s="7" t="s">
+      <c r="Q14" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="22" t="s">
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="U14" s="20"/>
+      <c r="U14" s="8" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6" t="s">
@@ -1466,11 +1498,11 @@
       <c r="B15" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="1" t="s">
         <v>3</v>
       </c>
@@ -1484,7 +1516,7 @@
       <c r="J15" s="4">
         <v>10</v>
       </c>
-      <c r="K15" s="16"/>
+      <c r="K15" s="14"/>
       <c r="L15" s="5">
         <v>15</v>
       </c>
@@ -1500,10 +1532,10 @@
       <c r="P15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="U15" s="20"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="U15" s="7"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6" t="s">
@@ -1512,11 +1544,11 @@
       <c r="B16" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
       <c r="F16" s="1" t="s">
         <v>3</v>
       </c>
@@ -1530,7 +1562,7 @@
       <c r="J16" s="4">
         <v>11</v>
       </c>
-      <c r="K16" s="16"/>
+      <c r="K16" s="14"/>
       <c r="L16" s="5">
         <v>14</v>
       </c>
@@ -1546,15 +1578,15 @@
       <c r="P16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q16" s="7" t="s">
+      <c r="Q16" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="22" t="s">
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="U16" s="20"/>
+      <c r="U16" s="7"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="6" t="s">
@@ -1563,11 +1595,11 @@
       <c r="B17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
       <c r="F17" s="1" t="s">
         <v>3</v>
       </c>
@@ -1581,7 +1613,7 @@
       <c r="J17" s="4">
         <v>12</v>
       </c>
-      <c r="K17" s="16"/>
+      <c r="K17" s="14"/>
       <c r="L17" s="5">
         <v>13</v>
       </c>
@@ -1595,15 +1627,15 @@
       <c r="P17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="U17" s="20"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="U17" s="7"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
       <c r="F18" s="1"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1611,7 +1643,7 @@
       <c r="J18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K18" s="16"/>
+      <c r="K18" s="14"/>
       <c r="L18" s="5" t="s">
         <v>0</v>
       </c>
@@ -1619,10 +1651,10 @@
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="3"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="U18" s="20"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="U18" s="7"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
@@ -1631,11 +1663,11 @@
       <c r="B19" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
       <c r="F19" s="1" t="s">
         <v>3</v>
       </c>
@@ -1651,7 +1683,7 @@
       <c r="J19" s="4">
         <v>24</v>
       </c>
-      <c r="K19" s="16"/>
+      <c r="K19" s="14"/>
       <c r="L19" s="5">
         <v>41</v>
       </c>
@@ -1661,15 +1693,17 @@
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="3"/>
-      <c r="Q19" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
+      <c r="Q19" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
       <c r="T19" t="s">
         <v>117</v>
       </c>
-      <c r="U19" s="20"/>
+      <c r="U19" s="7" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
@@ -1678,11 +1712,11 @@
       <c r="B20" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="1" t="s">
         <v>3</v>
       </c>
@@ -1698,7 +1732,7 @@
       <c r="J20" s="4">
         <v>25</v>
       </c>
-      <c r="K20" s="16"/>
+      <c r="K20" s="14"/>
       <c r="L20" s="5">
         <v>40</v>
       </c>
@@ -1708,15 +1742,15 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="3"/>
-      <c r="Q20" s="7" t="s">
+      <c r="Q20" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
       <c r="T20" t="s">
         <v>117</v>
       </c>
-      <c r="U20" s="20"/>
+      <c r="U20" s="7"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
@@ -1725,11 +1759,11 @@
       <c r="B21" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="1"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
@@ -1741,7 +1775,7 @@
       <c r="J21" s="4">
         <v>26</v>
       </c>
-      <c r="K21" s="16"/>
+      <c r="K21" s="14"/>
       <c r="L21" s="5">
         <v>39</v>
       </c>
@@ -1755,19 +1789,19 @@
         <v>11</v>
       </c>
       <c r="P21" s="3"/>
-      <c r="Q21" s="7" t="s">
+      <c r="Q21" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
       <c r="T21" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="1"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
@@ -1779,7 +1813,7 @@
       <c r="J22" s="4">
         <v>27</v>
       </c>
-      <c r="K22" s="16"/>
+      <c r="K22" s="14"/>
       <c r="L22" s="5">
         <v>38</v>
       </c>
@@ -1793,19 +1827,19 @@
         <v>12</v>
       </c>
       <c r="P22" s="3"/>
-      <c r="Q22" s="7" t="s">
+      <c r="Q22" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
       <c r="T22" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
       <c r="F23" s="1" t="s">
         <v>3</v>
       </c>
@@ -1817,7 +1851,7 @@
       <c r="J23" s="4">
         <v>28</v>
       </c>
-      <c r="K23" s="16"/>
+      <c r="K23" s="14"/>
       <c r="L23" s="5">
         <v>37</v>
       </c>
@@ -1829,11 +1863,11 @@
       <c r="P23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q23" s="7" t="s">
+      <c r="Q23" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
       <c r="T23" t="s">
         <v>118</v>
       </c>
@@ -1842,9 +1876,9 @@
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="1" t="s">
         <v>3</v>
       </c>
@@ -1856,7 +1890,7 @@
       <c r="J24" s="4">
         <v>29</v>
       </c>
-      <c r="K24" s="16"/>
+      <c r="K24" s="14"/>
       <c r="L24" s="5">
         <v>36</v>
       </c>
@@ -1868,11 +1902,11 @@
       <c r="P24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q24" s="7" t="s">
+      <c r="Q24" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
       <c r="T24" t="s">
         <v>94</v>
       </c>
@@ -1881,9 +1915,9 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="1"/>
       <c r="G25" s="2" t="s">
         <v>19</v>
@@ -1893,7 +1927,7 @@
       <c r="J25" s="4">
         <v>30</v>
       </c>
-      <c r="K25" s="16"/>
+      <c r="K25" s="14"/>
       <c r="L25" s="5">
         <v>35</v>
       </c>
@@ -1903,14 +1937,14 @@
       </c>
       <c r="O25" s="2"/>
       <c r="P25" s="3"/>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="7"/>
-      <c r="S25" s="7"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
       <c r="F26" s="1"/>
       <c r="G26" s="2" t="s">
         <v>20</v>
@@ -1920,7 +1954,7 @@
       <c r="J26" s="4">
         <v>31</v>
       </c>
-      <c r="K26" s="16"/>
+      <c r="K26" s="14"/>
       <c r="L26" s="5">
         <v>34</v>
       </c>
@@ -1930,14 +1964,14 @@
       </c>
       <c r="O26" s="2"/>
       <c r="P26" s="3"/>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="7"/>
-      <c r="S26" s="7"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
       <c r="F27" s="1"/>
       <c r="G27" s="2" t="s">
         <v>21</v>
@@ -1947,7 +1981,7 @@
       <c r="J27" s="4">
         <v>32</v>
       </c>
-      <c r="K27" s="17"/>
+      <c r="K27" s="15"/>
       <c r="L27" s="5">
         <v>33</v>
       </c>
@@ -1959,9 +1993,9 @@
       <c r="P27" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="U28" t="s">
@@ -1990,18 +2024,27 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="T11:T12"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F2:P3"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="Q2:S3"/>
+    <mergeCell ref="C2:E3"/>
+    <mergeCell ref="Q11:S12"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="Q25:S25"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="Q8:S8"/>
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C25:E25"/>
@@ -2018,31 +2061,22 @@
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F2:P3"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="Q2:S3"/>
-    <mergeCell ref="C2:E3"/>
-    <mergeCell ref="Q11:S12"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="Q22:S22"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="Q25:S25"/>
-    <mergeCell ref="Q26:S26"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated teensy io map
</commit_message>
<xml_diff>
--- a/Teensy IO Map.xlsx
+++ b/Teensy IO Map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dcecee288486a0d5/Documents/Arduino/BEV_2021_Teensy_Firmware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{CAC71B1E-86C1-4C54-AEDC-DA1FE7FE0A7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A7C5CCF0-D951-41F3-A134-FE8941946192}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{CAC71B1E-86C1-4C54-AEDC-DA1FE7FE0A7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4E653752-D9CD-4A54-B106-261EA0581C95}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3015" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="122">
   <si>
     <t>GND</t>
   </si>
@@ -309,12 +309,6 @@
     <t>0-5V</t>
   </si>
   <si>
-    <t>0-12V</t>
-  </si>
-  <si>
-    <t>0-5?</t>
-  </si>
-  <si>
     <t>speaker</t>
   </si>
   <si>
@@ -405,7 +399,7 @@
     <t>wheel move out</t>
   </si>
   <si>
-    <t>12v</t>
+    <t>0-12</t>
   </si>
 </sst>
 </file>
@@ -647,24 +641,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -684,6 +660,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -969,7 +963,7 @@
   <dimension ref="A2:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13:U14"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -979,51 +973,51 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="11" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="16" t="s">
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
       <c r="U2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="9" t="s">
@@ -1038,7 +1032,7 @@
       <c r="J4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="13"/>
+      <c r="K4" s="17"/>
       <c r="L4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1073,7 +1067,7 @@
       <c r="J5" s="4">
         <v>0</v>
       </c>
-      <c r="K5" s="14"/>
+      <c r="K5" s="18"/>
       <c r="L5" s="5" t="s">
         <v>0</v>
       </c>
@@ -1106,7 +1100,7 @@
       <c r="J6" s="4">
         <v>1</v>
       </c>
-      <c r="K6" s="14"/>
+      <c r="K6" s="18"/>
       <c r="L6" s="5" t="s">
         <v>1</v>
       </c>
@@ -1122,7 +1116,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
         <v>90</v>
@@ -1143,7 +1137,7 @@
       <c r="J7" s="4">
         <v>2</v>
       </c>
-      <c r="K7" s="14"/>
+      <c r="K7" s="18"/>
       <c r="L7" s="5">
         <v>23</v>
       </c>
@@ -1160,23 +1154,23 @@
         <v>3</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
-      <c r="T7" s="10" t="s">
-        <v>115</v>
+      <c r="T7" s="22" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -1191,7 +1185,7 @@
       <c r="J8" s="4">
         <v>3</v>
       </c>
-      <c r="K8" s="14"/>
+      <c r="K8" s="18"/>
       <c r="L8" s="5">
         <v>22</v>
       </c>
@@ -1206,21 +1200,21 @@
         <v>3</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
-      <c r="T8" s="10"/>
+      <c r="T8" s="22"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -1235,7 +1229,7 @@
       <c r="J9" s="4">
         <v>4</v>
       </c>
-      <c r="K9" s="14"/>
+      <c r="K9" s="18"/>
       <c r="L9" s="5">
         <v>21</v>
       </c>
@@ -1250,23 +1244,23 @@
       </c>
       <c r="P9" s="3"/>
       <c r="Q9" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
       <c r="T9" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="U9" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -1281,7 +1275,7 @@
       <c r="J10" s="4">
         <v>5</v>
       </c>
-      <c r="K10" s="14"/>
+      <c r="K10" s="18"/>
       <c r="L10" s="5">
         <v>20</v>
       </c>
@@ -1296,23 +1290,23 @@
       </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
       <c r="T10" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="U10" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -1327,7 +1321,7 @@
       <c r="J11" s="4">
         <v>6</v>
       </c>
-      <c r="K11" s="14"/>
+      <c r="K11" s="18"/>
       <c r="L11" s="5">
         <v>19</v>
       </c>
@@ -1341,24 +1335,24 @@
       <c r="P11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q11" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="R11" s="18"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="10" t="s">
-        <v>116</v>
+      <c r="Q11" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="R11" s="12"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="22" t="s">
+        <v>114</v>
       </c>
       <c r="U11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -1375,7 +1369,7 @@
       <c r="J12" s="4">
         <v>7</v>
       </c>
-      <c r="K12" s="14"/>
+      <c r="K12" s="18"/>
       <c r="L12" s="5">
         <v>18</v>
       </c>
@@ -1389,17 +1383,17 @@
       <c r="P12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="22"/>
-      <c r="T12" s="10"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="22"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -1416,7 +1410,7 @@
       <c r="J13" s="4">
         <v>8</v>
       </c>
-      <c r="K13" s="14"/>
+      <c r="K13" s="18"/>
       <c r="L13" s="5">
         <v>17</v>
       </c>
@@ -1431,15 +1425,15 @@
       </c>
       <c r="P13" s="3"/>
       <c r="Q13" s="9" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="R13" s="9"/>
       <c r="S13" s="9"/>
       <c r="T13" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="U13" s="8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -1447,7 +1441,7 @@
         <v>90</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>85</v>
@@ -1465,7 +1459,7 @@
       <c r="J14" s="4">
         <v>9</v>
       </c>
-      <c r="K14" s="14"/>
+      <c r="K14" s="18"/>
       <c r="L14" s="5">
         <v>16</v>
       </c>
@@ -1480,15 +1474,15 @@
       </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="9" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="R14" s="9"/>
       <c r="S14" s="9"/>
       <c r="T14" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="U14" s="8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -1496,7 +1490,7 @@
         <v>90</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>86</v>
@@ -1516,7 +1510,7 @@
       <c r="J15" s="4">
         <v>10</v>
       </c>
-      <c r="K15" s="14"/>
+      <c r="K15" s="18"/>
       <c r="L15" s="5">
         <v>15</v>
       </c>
@@ -1542,7 +1536,7 @@
         <v>90</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>87</v>
@@ -1562,7 +1556,7 @@
       <c r="J16" s="4">
         <v>11</v>
       </c>
-      <c r="K16" s="14"/>
+      <c r="K16" s="18"/>
       <c r="L16" s="5">
         <v>14</v>
       </c>
@@ -1579,12 +1573,12 @@
         <v>3</v>
       </c>
       <c r="Q16" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R16" s="9"/>
       <c r="S16" s="9"/>
       <c r="T16" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="U16" s="7"/>
     </row>
@@ -1593,7 +1587,7 @@
         <v>90</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>88</v>
@@ -1613,7 +1607,7 @@
       <c r="J17" s="4">
         <v>12</v>
       </c>
-      <c r="K17" s="14"/>
+      <c r="K17" s="18"/>
       <c r="L17" s="5">
         <v>13</v>
       </c>
@@ -1643,7 +1637,7 @@
       <c r="J18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K18" s="14"/>
+      <c r="K18" s="18"/>
       <c r="L18" s="5" t="s">
         <v>0</v>
       </c>
@@ -1658,13 +1652,13 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -1683,7 +1677,7 @@
       <c r="J19" s="4">
         <v>24</v>
       </c>
-      <c r="K19" s="14"/>
+      <c r="K19" s="18"/>
       <c r="L19" s="5">
         <v>41</v>
       </c>
@@ -1694,26 +1688,26 @@
       <c r="O19" s="2"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="R19" s="9"/>
       <c r="S19" s="9"/>
       <c r="T19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="U19" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -1732,7 +1726,7 @@
       <c r="J20" s="4">
         <v>25</v>
       </c>
-      <c r="K20" s="14"/>
+      <c r="K20" s="18"/>
       <c r="L20" s="5">
         <v>40</v>
       </c>
@@ -1743,24 +1737,26 @@
       <c r="O20" s="2"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="9" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
       <c r="T20" t="s">
-        <v>117</v>
-      </c>
-      <c r="U20" s="7"/>
+        <v>115</v>
+      </c>
+      <c r="U20" s="7" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -1775,7 +1771,7 @@
       <c r="J21" s="4">
         <v>26</v>
       </c>
-      <c r="K21" s="14"/>
+      <c r="K21" s="18"/>
       <c r="L21" s="5">
         <v>39</v>
       </c>
@@ -1790,16 +1786,24 @@
       </c>
       <c r="P21" s="3"/>
       <c r="Q21" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
       <c r="T21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="C22" s="9"/>
+      <c r="A22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>110</v>
+      </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="1"/>
@@ -1813,7 +1817,7 @@
       <c r="J22" s="4">
         <v>27</v>
       </c>
-      <c r="K22" s="14"/>
+      <c r="K22" s="18"/>
       <c r="L22" s="5">
         <v>38</v>
       </c>
@@ -1828,12 +1832,12 @@
       </c>
       <c r="P22" s="3"/>
       <c r="Q22" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R22" s="9"/>
       <c r="S22" s="9"/>
       <c r="T22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -1851,7 +1855,7 @@
       <c r="J23" s="4">
         <v>28</v>
       </c>
-      <c r="K23" s="14"/>
+      <c r="K23" s="18"/>
       <c r="L23" s="5">
         <v>37</v>
       </c>
@@ -1864,15 +1868,15 @@
         <v>3</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
       <c r="T23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="U23" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -1890,7 +1894,7 @@
       <c r="J24" s="4">
         <v>29</v>
       </c>
-      <c r="K24" s="14"/>
+      <c r="K24" s="18"/>
       <c r="L24" s="5">
         <v>36</v>
       </c>
@@ -1903,15 +1907,15 @@
         <v>3</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
       <c r="T24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="U24" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -1927,7 +1931,7 @@
       <c r="J25" s="4">
         <v>30</v>
       </c>
-      <c r="K25" s="14"/>
+      <c r="K25" s="18"/>
       <c r="L25" s="5">
         <v>35</v>
       </c>
@@ -1954,7 +1958,7 @@
       <c r="J26" s="4">
         <v>31</v>
       </c>
-      <c r="K26" s="14"/>
+      <c r="K26" s="18"/>
       <c r="L26" s="5">
         <v>34</v>
       </c>
@@ -1981,7 +1985,7 @@
       <c r="J27" s="4">
         <v>32</v>
       </c>
-      <c r="K27" s="15"/>
+      <c r="K27" s="19"/>
       <c r="L27" s="5">
         <v>33</v>
       </c>
@@ -1999,31 +2003,80 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="U28" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="U29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="U30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="U31" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="U30" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="U31" t="s">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="U32" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="U32" t="s">
-        <v>104</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="56">
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F2:P3"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="K4:K27"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="Q8:S8"/>
     <mergeCell ref="Q27:S27"/>
     <mergeCell ref="Q2:S3"/>
     <mergeCell ref="C2:E3"/>
@@ -2040,43 +2093,6 @@
     <mergeCell ref="Q18:S18"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="K4:K27"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F2:P3"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="T11:T12"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>